<commit_message>
update and lock quiz data spreadsheets
</commit_message>
<xml_diff>
--- a/sobotify/apps/quiz/quiz_english.xlsx
+++ b/sobotify/apps/quiz/quiz_english.xlsx
@@ -86,7 +86,7 @@
     <t xml:space="preserve">farewell</t>
   </si>
   <si>
-    <t xml:space="preserve">Thank you for taking part in the this quiz. </t>
+    <t xml:space="preserve">Thank you for taking part in this quiz. </t>
   </si>
   <si>
     <t xml:space="preserve">correct</t>
@@ -116,7 +116,7 @@
     <t xml:space="preserve">original question</t>
   </si>
   <si>
-    <t xml:space="preserve">What is result of 12 time 4?</t>
+    <t xml:space="preserve">What is the result of 12 time 4?</t>
   </si>
   <si>
     <t xml:space="preserve">repeated question/hint</t>
@@ -149,7 +149,7 @@
     <t xml:space="preserve">AND expected answer 4</t>
   </si>
   <si>
-    <t xml:space="preserve">Please name a shapes with 4 corners and a shape with 3 corners</t>
+    <t xml:space="preserve">Please name a shape with 4 corners and a shape with 3 corners</t>
   </si>
   <si>
     <t xml:space="preserve">shapes with 4 corners and 3 corners</t>
@@ -223,11 +223,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -246,12 +247,6 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -370,27 +365,27 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -398,7 +393,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -406,7 +401,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -494,14 +489,14 @@
   <dimension ref="A1:L520"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O20" activeCellId="0" sqref="O20"/>
+      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.4"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="3" min="3" style="2" width="23.44"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="3" min="3" style="2" width="23.43"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="4" min="4" style="2" width="23.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="88.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="12.03"/>
@@ -11194,13 +11189,14 @@
       <c r="L520" s="6"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <dataValidations count="4">
     <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C12:C17 C22:C28 C32:C38 C42:C48 C52:C58 C62:C68 C72:C78 C82:C88 C92:C98 C102:C108 C112:C118 C122:C128 C132:C138 C142:C148 C152:C158 C162:C168 C172:C178 C182:C188 C192:C198 C202:C208 C212:C218 C222:C228 C232:C238 C242:C248 C252:C258 C262:C268 C272:C278 C282:C288 C292:C298 C302:C308 C312:C318 C322:C328 C332:C338 C342:C348 C352:C358 C362:C368 C372:C378 C382:C388 C392:C398 C402:C408 C412:C418 C422:C428 C432:C438 C442:C448 C452:C458 C462:C468 C472:C478 C482:C488 C492:C498 C502:C508 C512:C518" type="list">
       <formula1>Settings!$B$2:$B$101</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C18:E20 E22:L30 C29:D30 E32:L40 C39:D40 E42:L50 C49:D50 E52:L60 C59:D60 E62:L70 C69:D70 E72:L80 C79:D80 E82:L90 C89:D90 E92:L100 C99:D100 E102:L110 C109:D110 E112:L120 C119:D120 E122:L130 C129:D130 E132:L140 C139:D140 E142:L150 C149:D150 E152:L160 C159:D160 E162:L170 C169:D170 E172:L180 C179:D180 E182:L190 C189:D190 E192:L200 C199:D200 E202:L210 C209:D210 E212:L220 C219:D220 E222:L230 C229:D230 E232:L240 C239:D240 E242:L250 C249:D250 E252:L260 C259:D260 E262:L270 C269:D270 E272:L280 C279:D280 E282:L290 C289:D290 E292:L300 C299:D300 E302:L310 C309:D310 E312:L320 C319:D320 E322:L330 C329:D330 E332:L340 C339:D340 E342:L350 C349:D350 E352:L360 C359:D360 E362:L370 C369:D370 E372:L380 C379:D380 E382:L390 C389:D390 E392:L400 C399:D400 E402:L410 C409:D410 E412:L420 C419:D420 E422:L430 C429:D430 E432:L440 C439:D440 E442:L450 C449:D450 E452:L460 C459:D460 E462:L470 C469:D470 E472:L480 C479:D480 E482:L490 C489:D490 E492:L500 C499:D500 E502:L510 C509:D510 E512:L520 C519:D520" type="none">
-      <formula1>#REF!</formula1>
+      <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D12:D17 D22:D28 D32:D38 D42:D48 D52:D58 D62:D68 D72:D78 D82:D88 D92:D98 D102:D108 D112:D118 D122:D128 D132:D138 D142:D148 D152:D158 D162:D168 D172:D178 D182:D188 D192:D198 D202:D208 D212:D218 D222:D228 D232:D238 D242:D248 D252:D258 D262:D268 D272:D278 D282:D288 D292:D298 D302:D308 D312:D318 D322:D328 D332:D338 D342:D348 D352:D358 D362:D368 D372:D378 D382:D388 D392:D398 D402:D408 D412:D418 D422:D428 D432:D438 D442:D448 D452:D458 D462:D468 D472:D478 D482:D488 D492:D498 D502:D508 D512:D518" type="whole">
@@ -11233,7 +11229,7 @@
       <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="18" t="s">
@@ -11244,7 +11240,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="16" t="s">
@@ -11252,7 +11248,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="17" t="s">
         <v>61</v>
       </c>
       <c r="B3" s="16" t="s">
@@ -11556,9 +11552,10 @@
       <c r="B101" s="16"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <dataValidations count="1">
     <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:B3 B4:B101" type="none">
-      <formula1>#REF!</formula1>
+      <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>